<commit_message>
Agregar datos a plantilla calendario de pagos.
</commit_message>
<xml_diff>
--- a/nomina/docs_plantillas/Plantilla_Calendario_de_Pagos.xlsx
+++ b/nomina/docs_plantillas/Plantilla_Calendario_de_Pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerardo\Documents\INAES\repositorio\SIA_V2\nomina\docs_plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA4EA17-7E94-4E61-886B-063A3964BD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B09A86-918E-49C8-888F-FC1B28DFD50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1er_Trim" sheetId="7" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>1ª QUINCENA</t>
   </si>
   <si>
     <t>2ª QUINCENA</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>MES</t>
@@ -393,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -431,15 +428,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -563,6 +552,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13040,8 +13032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13067,233 +13059,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="2" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
-    </row>
-    <row r="2" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
       <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
+    </row>
+    <row r="4" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="53"/>
+    </row>
+    <row r="5" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="34"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="43"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="43"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5" s="43"/>
+      <c r="X5" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="55"/>
-    </row>
-    <row r="5" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="38" t="s">
+    <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="44" t="s">
-        <v>23</v>
+      <c r="K6" s="46"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="45" t="s">
+        <v>4</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="44" t="s">
-        <v>27</v>
+      <c r="N6" s="46"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="45" t="s">
+        <v>4</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="44" t="s">
-        <v>26</v>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="45" t="s">
+        <v>4</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="44" t="s">
-        <v>31</v>
+      <c r="T6" s="46"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="45" t="s">
+        <v>4</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="45"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="W5" s="45"/>
-      <c r="X5" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="47"/>
     </row>
-    <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="47" t="s">
+    <row r="7" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="48"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="47" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="48"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="47" t="s">
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="47" t="s">
+      <c r="Q7" s="49"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="48"/>
-      <c r="U6" s="49"/>
-      <c r="V6" s="47" t="s">
+      <c r="T7" s="49"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="W6" s="48"/>
-      <c r="X6" s="49"/>
-    </row>
-    <row r="7" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="51"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="T7" s="51"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="W7" s="51"/>
-      <c r="X7" s="52"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="50"/>
     </row>
     <row r="9" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -13322,41 +13314,32 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>19</v>
+      <c r="A10" s="26" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E10" s="14"/>
       <c r="F10" s="15"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="27"/>
+      <c r="J10" s="13"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="13"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="13"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="13"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="13"/>
+      <c r="X10" s="25"/>
     </row>
     <row r="11" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
@@ -13382,7 +13365,7 @@
       <c r="X11" s="20"/>
     </row>
     <row r="12" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
@@ -13408,36 +13391,27 @@
       <c r="X12" s="10"/>
     </row>
     <row r="13" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="27"/>
+      <c r="J13" s="13"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="13"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="13"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="13"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="13"/>
+      <c r="X13" s="25"/>
     </row>
     <row r="14" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -13493,41 +13467,32 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>20</v>
+      <c r="A17" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E17" s="14"/>
       <c r="F17" s="21"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="27"/>
+      <c r="J17" s="13"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="13"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="13"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="13"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="13"/>
+      <c r="X17" s="25"/>
     </row>
     <row r="18" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="16"/>
       <c r="C18" s="17"/>
       <c r="D18" s="18"/>
@@ -13553,7 +13518,7 @@
       <c r="X18" s="20"/>
     </row>
     <row r="19" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -13579,36 +13544,27 @@
       <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H20" s="14"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="27"/>
+      <c r="J20" s="13"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="13"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="13"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="13"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="13"/>
+      <c r="X20" s="25"/>
     </row>
     <row r="21" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
@@ -13664,41 +13620,32 @@
       <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>21</v>
+      <c r="A24" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="E24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H24" s="14"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="27"/>
+      <c r="J24" s="13"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="13"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="13"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="13"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="13"/>
+      <c r="X24" s="25"/>
     </row>
     <row r="25" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
@@ -13724,7 +13671,7 @@
       <c r="X25" s="20"/>
     </row>
     <row r="26" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
@@ -13750,36 +13697,27 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="15"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="27"/>
+      <c r="J27" s="13"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="13"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="13"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="13"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="13"/>
+      <c r="X27" s="25"/>
     </row>
     <row r="28" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -13815,44 +13753,32 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C60" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="V27:X27"/>
+  <mergeCells count="16">
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A24:A27"/>
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A3:X3"/>
     <mergeCell ref="A2:X2"/>
@@ -13863,27 +13789,9 @@
     <mergeCell ref="J5:L7"/>
     <mergeCell ref="M5:O7"/>
     <mergeCell ref="P5:R7"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J27:L27"/>
     <mergeCell ref="A4:X4"/>
     <mergeCell ref="S5:U7"/>
     <mergeCell ref="V5:X7"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="S27:U27"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -13899,7 +13807,7 @@
   <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:X4"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13925,220 +13833,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
-    </row>
-    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>22</v>
+      <c r="A3" s="30" t="s">
+        <v>21</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="34"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
     <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="str">
+      <c r="A4" s="51" t="str">
         <f>'1er_Trim'!A4:X4</f>
         <v>CALENDARIO  DE  PAGOS  DE  NOMINA  DEL  %PERIODO%</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="55"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="53"/>
     </row>
     <row r="5" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="str">
+      <c r="A5" s="33" t="str">
         <f>'1er_Trim'!A5:A7</f>
         <v>MES</v>
       </c>
-      <c r="B5" s="38" t="str">
+      <c r="B5" s="36" t="str">
         <f>'1er_Trim'!B5:C7</f>
         <v>CONCEPTO</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="44" t="str">
+      <c r="C5" s="37"/>
+      <c r="D5" s="42" t="str">
         <f>'1er_Trim'!D5:F7</f>
         <v>ENTREGA DE INFORMACION A LA SUB. ADMON. SDOS.</v>
       </c>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="44" t="str">
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="42" t="str">
         <f>'1er_Trim'!G5:I7</f>
         <v>ELABORACION DE LA NOMINA</v>
       </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="44" t="str">
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="42" t="str">
         <f>'1er_Trim'!J5:L7</f>
         <v>ENTREGA DEL ARCHIVO DE NOMINA A LA DIR. PRES. Y CONTAB.</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="44" t="str">
+      <c r="K5" s="54"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="42" t="str">
         <f>'1er_Trim'!M5:O7</f>
         <v>ENTREGA DE INTERFASE AL AREA DE TESORERIA</v>
       </c>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="44" t="s">
+      <c r="N5" s="54"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="56"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="44" t="str">
+      <c r="T5" s="54"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="42" t="str">
         <f>'1er_Trim'!V5:X7</f>
         <v>FECHA DE PAGO</v>
       </c>
-      <c r="W5" s="56"/>
-      <c r="X5" s="57"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="55"/>
     </row>
     <row r="6" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="60"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="58"/>
     </row>
     <row r="7" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="61"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="63"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
     </row>
     <row r="9" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -14167,41 +14075,37 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>7</v>
+      <c r="A10" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E10" s="14"/>
       <c r="F10" s="15"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="27"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
@@ -14227,7 +14131,7 @@
       <c r="X11" s="20"/>
     </row>
     <row r="12" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
@@ -14253,36 +14157,32 @@
       <c r="X12" s="10"/>
     </row>
     <row r="13" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="27"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="67"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="67"/>
+      <c r="W13" s="68"/>
+      <c r="X13" s="69"/>
     </row>
     <row r="14" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -14338,41 +14238,37 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>8</v>
+      <c r="A17" s="26" t="s">
+        <v>7</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="27"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="68"/>
+      <c r="X17" s="69"/>
     </row>
     <row r="18" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="16"/>
       <c r="C18" s="17"/>
       <c r="D18" s="18"/>
@@ -14398,7 +14294,7 @@
       <c r="X18" s="20"/>
     </row>
     <row r="19" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -14424,36 +14320,32 @@
       <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H20" s="14"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="27"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="68"/>
+      <c r="X20" s="69"/>
     </row>
     <row r="21" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
@@ -14509,41 +14401,37 @@
       <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>9</v>
+      <c r="A24" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="E24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H24" s="14"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="27"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="67"/>
+      <c r="W24" s="68"/>
+      <c r="X24" s="69"/>
     </row>
     <row r="25" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
@@ -14569,7 +14457,7 @@
       <c r="X25" s="20"/>
     </row>
     <row r="26" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
@@ -14595,36 +14483,32 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="15"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="27"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="68"/>
+      <c r="R27" s="69"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="69"/>
+      <c r="V27" s="67"/>
+      <c r="W27" s="68"/>
+      <c r="X27" s="69"/>
     </row>
     <row r="28" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -14660,12 +14544,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -14681,7 +14565,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="16">
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A2:X2"/>
     <mergeCell ref="A3:X3"/>
@@ -14696,38 +14580,8 @@
     <mergeCell ref="S5:U7"/>
     <mergeCell ref="V5:X7"/>
     <mergeCell ref="A24:A27"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J20:L20"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A17:A20"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="V27:X27"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -14742,8 +14596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11:AE12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14769,220 +14623,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
-    </row>
-    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>22</v>
+      <c r="A3" s="30" t="s">
+        <v>21</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="34"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
     <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="str">
+      <c r="A4" s="51" t="str">
         <f>'1er_Trim'!A4:X4</f>
         <v>CALENDARIO  DE  PAGOS  DE  NOMINA  DEL  %PERIODO%</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="55"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="53"/>
     </row>
     <row r="5" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="str">
+      <c r="A5" s="33" t="str">
         <f>'1er_Trim'!A5:A7</f>
         <v>MES</v>
       </c>
-      <c r="B5" s="38" t="str">
+      <c r="B5" s="36" t="str">
         <f>'1er_Trim'!B5:C7</f>
         <v>CONCEPTO</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="44" t="str">
+      <c r="C5" s="37"/>
+      <c r="D5" s="42" t="str">
         <f>'1er_Trim'!D5:F7</f>
         <v>ENTREGA DE INFORMACION A LA SUB. ADMON. SDOS.</v>
       </c>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="44" t="str">
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="42" t="str">
         <f>'1er_Trim'!G5:I7</f>
         <v>ELABORACION DE LA NOMINA</v>
       </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="44" t="str">
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="42" t="str">
         <f>'1er_Trim'!J5:L7</f>
         <v>ENTREGA DEL ARCHIVO DE NOMINA A LA DIR. PRES. Y CONTAB.</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="44" t="str">
+      <c r="K5" s="54"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="42" t="str">
         <f>'1er_Trim'!M5:O7</f>
         <v>ENTREGA DE INTERFASE AL AREA DE TESORERIA</v>
       </c>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="44" t="s">
+      <c r="N5" s="54"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="56"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="44" t="str">
+      <c r="T5" s="54"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="42" t="str">
         <f>'1er_Trim'!V5:X7</f>
         <v>FECHA DE PAGO</v>
       </c>
-      <c r="W5" s="56"/>
-      <c r="X5" s="57"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="55"/>
     </row>
     <row r="6" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="60"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="58"/>
     </row>
     <row r="7" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="61"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="63"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
     </row>
     <row r="9" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -15011,41 +14865,37 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>10</v>
+      <c r="A10" s="26" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E10" s="14"/>
       <c r="F10" s="15"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="27"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
@@ -15071,7 +14921,7 @@
       <c r="X11" s="20"/>
     </row>
     <row r="12" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
@@ -15097,36 +14947,32 @@
       <c r="X12" s="10"/>
     </row>
     <row r="13" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="27"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="67"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="67"/>
+      <c r="W13" s="68"/>
+      <c r="X13" s="69"/>
     </row>
     <row r="14" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -15182,41 +15028,37 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>11</v>
+      <c r="A17" s="26" t="s">
+        <v>10</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="27"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="68"/>
+      <c r="X17" s="69"/>
     </row>
     <row r="18" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="16"/>
       <c r="C18" s="17"/>
       <c r="D18" s="18"/>
@@ -15242,7 +15084,7 @@
       <c r="X18" s="20"/>
     </row>
     <row r="19" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -15268,36 +15110,32 @@
       <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H20" s="14"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="27"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="68"/>
+      <c r="X20" s="69"/>
     </row>
     <row r="21" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
@@ -15353,41 +15191,37 @@
       <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="64" t="s">
-        <v>12</v>
+      <c r="A24" s="62" t="s">
+        <v>11</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="E24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H24" s="14"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="27"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="67"/>
+      <c r="W24" s="68"/>
+      <c r="X24" s="69"/>
     </row>
     <row r="25" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="64"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
@@ -15413,7 +15247,7 @@
       <c r="X25" s="20"/>
     </row>
     <row r="26" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="64"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
@@ -15439,36 +15273,32 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="64"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="15"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="27"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="68"/>
+      <c r="R27" s="69"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="69"/>
+      <c r="V27" s="67"/>
+      <c r="W27" s="68"/>
+      <c r="X27" s="69"/>
     </row>
     <row r="28" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -15504,12 +15334,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -15525,7 +15355,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="16">
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A2:X2"/>
     <mergeCell ref="A3:X3"/>
@@ -15536,42 +15366,12 @@
     <mergeCell ref="P5:R7"/>
     <mergeCell ref="S5:U7"/>
     <mergeCell ref="V5:X7"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="V17:X17"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:C7"/>
     <mergeCell ref="D5:F7"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V27:X27"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J27:L27"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A24:A27"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M20:O20"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -15587,7 +15387,7 @@
   <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15613,221 +15413,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="2" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
-    </row>
-    <row r="2" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
     <row r="3" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>22</v>
+      <c r="A3" s="30" t="s">
+        <v>21</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="34"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
     <row r="4" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="str">
+      <c r="A4" s="51" t="str">
         <f>'1er_Trim'!A4:X4</f>
         <v>CALENDARIO  DE  PAGOS  DE  NOMINA  DEL  %PERIODO%</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="55"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="53"/>
     </row>
     <row r="5" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="str">
+      <c r="A5" s="33" t="str">
         <f>'1er_Trim'!A5:A7</f>
         <v>MES</v>
       </c>
-      <c r="B5" s="38" t="str">
+      <c r="B5" s="36" t="str">
         <f>'1er_Trim'!B5:C7</f>
         <v>CONCEPTO</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="44" t="str">
+      <c r="C5" s="37"/>
+      <c r="D5" s="42" t="str">
         <f>'1er_Trim'!D5:F7</f>
         <v>ENTREGA DE INFORMACION A LA SUB. ADMON. SDOS.</v>
       </c>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="44" t="str">
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="42" t="str">
         <f>'1er_Trim'!G5:I7</f>
         <v>ELABORACION DE LA NOMINA</v>
       </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="44" t="str">
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="42" t="str">
         <f>'1er_Trim'!J5:L7</f>
         <v>ENTREGA DEL ARCHIVO DE NOMINA A LA DIR. PRES. Y CONTAB.</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="44" t="str">
+      <c r="K5" s="54"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="42" t="str">
         <f>'1er_Trim'!M5:O7</f>
         <v>ENTREGA DE INTERFASE AL AREA DE TESORERIA</v>
       </c>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="44" t="s">
+      <c r="N5" s="54"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="56"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="44" t="str">
+      <c r="T5" s="54"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="42" t="str">
         <f>'1er_Trim'!V5:X7</f>
         <v>FECHA DE PAGO</v>
       </c>
-      <c r="W5" s="56"/>
-      <c r="X5" s="57"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="55"/>
     </row>
     <row r="6" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="60"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="58"/>
       <c r="AA6" s="22"/>
     </row>
     <row r="7" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="61"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="63"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
     </row>
     <row r="9" spans="1:30" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -15856,41 +15656,37 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:30" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>13</v>
+      <c r="A10" s="26" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E10" s="14"/>
       <c r="F10" s="15"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="27"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:30" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
@@ -15916,7 +15712,7 @@
       <c r="X11" s="20"/>
     </row>
     <row r="12" spans="1:30" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
@@ -15941,40 +15737,36 @@
       <c r="W12" s="9"/>
       <c r="X12" s="10"/>
       <c r="AD12" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="27"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="67"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="67"/>
+      <c r="W13" s="68"/>
+      <c r="X13" s="69"/>
     </row>
     <row r="14" spans="1:30" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -16030,41 +15822,37 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="68" t="s">
-        <v>14</v>
+      <c r="A17" s="66" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="27"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="68"/>
+      <c r="X17" s="69"/>
     </row>
     <row r="18" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="68"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="16"/>
       <c r="C18" s="17"/>
       <c r="D18" s="18"/>
@@ -16090,7 +15878,7 @@
       <c r="X18" s="20"/>
     </row>
     <row r="19" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="68"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -16116,36 +15904,32 @@
       <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="68"/>
+      <c r="A20" s="66"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H20" s="14"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="27"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="68"/>
+      <c r="X20" s="69"/>
     </row>
     <row r="21" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
@@ -16178,7 +15962,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
@@ -16203,46 +15987,42 @@
       <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="68" t="s">
-        <v>15</v>
+      <c r="A24" s="66" t="s">
+        <v>14</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="E24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H24" s="14"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="27"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="67"/>
+      <c r="W24" s="68"/>
+      <c r="X24" s="69"/>
     </row>
     <row r="25" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="68"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="67"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
       <c r="G25" s="18"/>
       <c r="H25" s="19"/>
       <c r="I25" s="20"/>
@@ -16263,7 +16043,7 @@
       <c r="X25" s="20"/>
     </row>
     <row r="26" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="68"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
@@ -16289,46 +16069,42 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="68"/>
+      <c r="A27" s="66"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="15"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="27"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="68"/>
+      <c r="R27" s="69"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="69"/>
+      <c r="V27" s="67"/>
+      <c r="W27" s="68"/>
+      <c r="X27" s="69"/>
     </row>
     <row r="28" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="16"/>
       <c r="C28" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="67"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="65"/>
       <c r="G28" s="18"/>
       <c r="H28" s="19"/>
       <c r="I28" s="20"/>
@@ -16356,12 +16132,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -16377,7 +16153,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="18">
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A2:X2"/>
     <mergeCell ref="A3:X3"/>
@@ -16391,41 +16167,11 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A24:A27"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M20:O20"/>
     <mergeCell ref="D25:F25"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="V17:X17"/>
     <mergeCell ref="P5:R7"/>
     <mergeCell ref="S5:U7"/>
     <mergeCell ref="V5:X7"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="V24:X24"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="V27:X27"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>